<commit_message>
update w/ Faith info
</commit_message>
<xml_diff>
--- a/Data/lhd_dir.xlsx
+++ b/Data/lhd_dir.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcheadle2/Box/GitHub/Software/R/RLifeHD/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DE88F5-12AB-8842-ABF4-0703A93403F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E025ED-4ED2-5841-BE3A-3DA8B0130397}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="-19800" windowWidth="28040" windowHeight="17440" xr2:uid="{1F93C3D2-1ECF-5B4C-B148-58E25BF9C04C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>hostname</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>Darwin</t>
+  </si>
+  <si>
+    <t>LookingGlass</t>
+  </si>
+  <si>
+    <t>/Users/fmdec/Box/Github/Research/</t>
+  </si>
+  <si>
+    <t>fmdec</t>
   </si>
 </sst>
 </file>
@@ -403,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C96B5B-A5A2-F54C-8244-37FD8A60420A}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,6 +469,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>